<commit_message>
Updated sample excel files for mongo insert
</commit_message>
<xml_diff>
--- a/mongodbInsertScript/placeShipMethodExcelFileHere/z_sampleShipMethod.xlsx
+++ b/mongodbInsertScript/placeShipMethodExcelFileHere/z_sampleShipMethod.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="21">
   <si>
     <t>UPC</t>
   </si>
@@ -56,6 +56,27 @@
   </si>
   <si>
     <t>aProd3</t>
+  </si>
+  <si>
+    <t>Package</t>
+  </si>
+  <si>
+    <t>Preparation</t>
+  </si>
+  <si>
+    <t>padded env1</t>
+  </si>
+  <si>
+    <t>padded env2</t>
+  </si>
+  <si>
+    <t>padded env3</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>Bubblewrap</t>
   </si>
 </sst>
 </file>
@@ -105,7 +126,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -141,6 +162,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -449,7 +471,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D10" sqref="D10"/>
+      <selection pane="bottomLeft" activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -459,7 +481,7 @@
     <col min="3" max="3" width="6.85546875" customWidth="1"/>
     <col min="4" max="4" width="21.7109375" customWidth="1"/>
     <col min="5" max="5" width="7.5703125" customWidth="1"/>
-    <col min="6" max="6" width="6.28515625" customWidth="1"/>
+    <col min="6" max="6" width="15" customWidth="1"/>
     <col min="7" max="8" width="10" customWidth="1"/>
   </cols>
   <sheetData>
@@ -479,8 +501,12 @@
       <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
+      <c r="F1" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="15" t="s">
+        <v>15</v>
+      </c>
       <c r="H1" s="4"/>
       <c r="I1" s="4"/>
       <c r="J1" s="4"/>
@@ -509,8 +535,12 @@
       <c r="E2" s="7">
         <v>1</v>
       </c>
-      <c r="F2" s="6"/>
-      <c r="G2" s="4"/>
+      <c r="F2" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" s="15" t="s">
+        <v>19</v>
+      </c>
       <c r="H2" s="4"/>
       <c r="I2" s="4"/>
       <c r="J2" s="4"/>
@@ -539,8 +569,12 @@
       <c r="E3" s="7">
         <v>16</v>
       </c>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
+      <c r="F3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" s="15" t="s">
+        <v>19</v>
+      </c>
       <c r="H3" s="4"/>
       <c r="I3" s="4"/>
       <c r="J3" s="4"/>
@@ -567,8 +601,12 @@
         <v>5</v>
       </c>
       <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
+      <c r="F4" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" s="15" t="s">
+        <v>20</v>
+      </c>
       <c r="H4" s="4"/>
       <c r="I4" s="4"/>
       <c r="J4" s="4"/>
@@ -595,8 +633,12 @@
         <v>6</v>
       </c>
       <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
+      <c r="F5" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>20</v>
+      </c>
       <c r="H5" s="4"/>
       <c r="I5" s="4"/>
       <c r="J5" s="4"/>

</xml_diff>